<commit_message>
no of files uploaded
</commit_message>
<xml_diff>
--- a/EmployeeResumeRead/employee_resumes_data.xlsx
+++ b/EmployeeResumeRead/employee_resumes_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,184 +468,1852 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mohitk</t>
+          <t>ajaikrishnan</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Name: Mohit Kumar</t>
+          <t xml:space="preserve">OBJECTIVE STATEMENT </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Email: mohitk9917@gm</t>
+          <t>Excel as a Senior We</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7983748491</t>
+          <t>9345211363</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>mohitk9917@gmail.com</t>
+          <t>ajaikrishnan13@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>MohitKumar</t>
+          <t>AjaiKrishnan</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rjtrivedi</t>
+          <t>anand</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RAJAT TRIVEDI</t>
+          <t>ANAND R</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Mob. No: 8851456225</t>
+          <t>UI DEVELOPER</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>8851456225</t>
+          <t>+91 9884254608</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>rjtrivedi0@gmail.com</t>
+          <t>anand0447@gmail.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>RajatTrivedi</t>
+          <t>Anand</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>rameshkeshari</t>
+          <t>arangasamy.arulselvi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Name RAMESH KUMAR KE</t>
+          <t>ARULSELVI. A</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>JobRole: SalesforceD</t>
+          <t xml:space="preserve">+91 9788781303      </t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9616671130</t>
+          <t>+91 9788781303</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>rameshkeshari9@gmail.com</t>
+          <t>arangasamy.arulselvi@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>RAMESHKUMARKESHARI</t>
+          <t>Arulselvi</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ravikiranrr</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ravikiran Rathod</t>
+          <t>NAME</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>MA (Master of Econom</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>8983735080</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>ravikiranrr443@gmail.com</t>
-        </is>
-      </c>
+          <t>BALASUBRAMANI P</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>RavikiranRathod</t>
+          <t>Balasubramani</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>bavithrarajagopal</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DEEPANK TIWARI</t>
+          <t>+91 9677627791</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Salesforce Developer</t>
+          <t>B A V I T H R A R</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>8889622055</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>+91 9677627791</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>bavithrarajagopal@gmail.com</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DeepankTiwari</t>
+          <t>BavithraRajagopal</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>shivagolla</t>
+          <t>bhuvanaapps</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Golla Shiva</t>
+          <t>3, Mariamman Kovil S</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t xml:space="preserve">Highly seasoned and </t>
+          <t>BHUVANESWARI N</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>7013874066</t>
+          <t>9940839951</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>shivagolla2023@gmail.com</t>
+          <t>bhuvanaapps1409@gmail.com</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>GollaShiva</t>
+          <t>BhuvaneswariNagarajan</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>chanderbalu</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>chanderbalu109@gmail</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9677184672</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>chanderbalu109@gmail.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>ChanderBalasubramanian</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>praveen.pec</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Praveen Kumar CH    </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Software Developer, </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>+91 9600179722</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>praveen.pec89@gmail.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Chevurupraveenkumar</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>chithambaramd</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CHITHAMBARAM. D</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         E-Mail: chi</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>chithambaramd85@gmail.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ChithambaramD</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>dhanasheelan</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Dhanasheelan Shanmug</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>React.js | JavaScrip</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>9566612764</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>dhanasheelan1994@gmail.com</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Dhanasheelans</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>elavarasan.selvaraj</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Elavarasan S</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Chennai, Tamil Nadu</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>9940837307</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>elavarasan.selvaraj14@gmail.com</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>ElavarasanS</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>epsinov</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>EPSI VICTORIYA</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Angular Developer &amp; </t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>epsinov23@gmail.com</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>EpsiVictoriya</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ganapathibabu</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>S.D. Ganesh Babu</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>E-Mail: - ganapathib</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>ganapathibabu@gmail.com</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>GaneshBabuSD</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>indusathiya</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Indumathi M</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Immediate Joiner. Ha</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>9789070160</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>indusathiya2015@gmail.com</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>IndumathiM</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>chenchaiah</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	J CHENCHAIH</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>WEB DEVELOPER</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>9491239138</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>chenchaiah16@gmail.com</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>JCHENCHAIAH</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>jagadeeswari.ece.</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Jagadeeswari s</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Mobile No: +91 93454</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>+91 9345481572</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>jagadeeswari.ece.27@gmail.com</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Jegadeeswari</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>bonsaikarthick</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>KARTHICK S</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>bonsaikarthick1991@g</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>9790475794</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>bonsaikarthick1991@gmail.com</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>KARTHICKS</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>karthihavocless</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>KARTHIKEYAN G</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>9094220219</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>karthihavocless28@gmail.com</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>KarthikeyanG</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>karthikpjk</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>KARTHIKEYANJ</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>SeniorFrontendDevelo</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>9578038358</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>karthikpjk@gmail.com</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>KARTHIKEYAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>manishj</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>MOBILE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>(+91) 9943420922</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>9943420922</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>manishj1597@gmail.com</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Manikandan</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>a.najeerudeen</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mohamed Najeerudeen </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>(Immediate Joiner) +</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>8072860050</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>a.najeerudeen@gmail.com</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MohamedNajeerudeenA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>mohannbtechit</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>MOHAN RAJ | FRONT-EN</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Chennai, India | +91</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>8056254846</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>mohannbtechit12@gmail.com</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>MOHANRAJ</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>mmugilan</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>MUGILAN.M | Phone: +</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>MUGILAN.M</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>+91 9500828236</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>mmugilan09@gmail.com</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>MugilanM</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>mugilanbarasan</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Mugil A</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Web Developer</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>8667486072</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>mugilanbarasan@gmail.com</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Mugil</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>nandhinics</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Nandhini Mani</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Chennai, India</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>+91 9843662916</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>nandhinics29@gmail.com</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>NandhiniMani</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>inijanthan</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NIJANTHAN I</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>9790814513</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>inijanthan@gmail.com</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>NijanthanI</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>nikks</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Nitish Kumar</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>SeniorFullStackDevel</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>+919790850233</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>nikks3768@gmail.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>NITISHKUMAR</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>paul.arockiyam</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Palraj Arockiaraj</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>paul.arockiyam@gmail</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>9840823280</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>paul.arockiyam@gmail.com</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>PalrajArockiaraj</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Pandiyarajan.tcps</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>WEB DEVELOPER</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PANDIYARAJAN.S      </t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>+91 6369773659</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Pandiyarajan.tcps@gmail.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>PANDIYARAJANS</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>prema</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Resume</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>of</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>7639425279</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>prema203@gmail.com</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Piraimathi</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>spradeebaselvaraj</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>S.PRADEEBA</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>S.PRADEEBA</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>7708752621</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>spradeebaselvaraj@gmail.com</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>pradeeba</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>mcapraveenkumarp</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>P. PRAVEEN KUMAR</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>+91 7845627408 </t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>+91 7845627408</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>mcapraveenkumarp@gmail.com</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>PraveenKumarP</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>ragulkrishnaraj</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Ragul Krishnaraj Mob</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>UI UX Developer &amp; De</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>9655334489</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>ragulkrishnaraj@gmail.com</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>RagulKrishnaraj</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ramlakshmibe</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Senior Web Developer</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Senior Web Developer</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>9884563003</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>ramlakshmibe@gmail.comAddress</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Ramalakshmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>devr</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>DEVENDIRAN R</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No.5/65, 2nd floor, </t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>9789896533</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>devr2086@gmail.com</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>RDevendiran</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>sajin</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>SAJIN PRABHU Y</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Email Id: sajin43@gm</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>9944682919</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>sajin43@gmail.com</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>SajinPrabhuY</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ahino.s</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>RESUME</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>SAM AHINO S</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>+91 6383449195</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ahino.s1@gmail.com</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>SamAhinoS</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>santhoshsac</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Santhosh Kumar C</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>7402239129</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>santhoshsac1994@gmail.com</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Santhoshkumar</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>tsanthoshkumar</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>SANTHOSH KUMAR T</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Contact</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>+91 7418882627</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>tsanthoshkumar06@gmail.com</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>SanthoshKumar</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>saravana</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Saravanan Balasubram</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>saravana282008@gmail</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>9840490629</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>saravana282008@gmail.com</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Saravanan</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>csathishkumar</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Name: Sathish Kumar </t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Email: csathishkumar</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>8220642057</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>csathishkumar217@gmail.com</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>SathishKumar</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>shaktishkumar</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Shaktish kumar M R</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>91766 83582</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>shaktishkumar@gmail.com</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>ShaktishkumarMR</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>shalu.ks</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SHALINI K S</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>SENIOR PROGRAMMER</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>7358756920</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>shalu05.ks@gmail.com</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>ShaliniKS</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>sengupta.shubodeep</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CONTACT</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>SHUBODEEP SENGUPTA</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>8949969210</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>sengupta.shubodeep@gmail.com</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Shubodeepsengupta</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>hasyms</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Plotno580,</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Shunmuga Sankar</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>8807640056</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>hasyms21@gmail.com</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>ShunmugaSankarM</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>shyamala.k.techie</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>SHYAMALA K</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Phone: +91-93619 541</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>shyamala.k.techie@gmail.com</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>ShyamalaK</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>hellosimbu</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SILAMBARASAN K</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>hellosimbu2023@gmail</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>+91 9360277878</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>hellosimbu2023@gmail.com</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>silambarsan</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>arivu</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SIVARAMAKRISHNAN D  </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    arivu1243@gmail.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>+91 9488672109</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>arivu1243@gmail.com</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>SivaramakrishnanD</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>keerthisuryakumar</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>S.Keerthiha</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>10-5-15 /A.9 Rathina</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>9597248302</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>keerthisuryakumar@gmail.com</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Skeerthiha</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>mailforsoundar</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>S.SOUNDAR RAJAN Emai</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Contact No: 99403623</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>9940362337</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>mailforsoundar@gmail.com</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>SoundarRajan</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>sujith.spk</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Sujith SoundaraPandi</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Handphone : +91 9363</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>+91 9363474903</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>sujith.spk46@hotmail.com</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>SujithSoundaraPandianK</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>surendrann</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>SURENDRAN N</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Senior UI Frontend D</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>9965470854</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>surendrann85@gmail.com</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>SURENDRANNATARAJAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>vasanth</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>VASANTHAN RAJI</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Email: vasanth100790</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>+91 7871797603</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>vasanth100790@gmail.com</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>VasanthanRaji</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>velmuruganc</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Professional Summary</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Skilled and motivate</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>+91 9360322734</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>velmuruganc6@gmail.com</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>VelmuruganC</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>velmurugantelecom</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>RESUME</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Velmurugan S Mail: v</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>6382974326</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>velmurugantelecom@gmail.com</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>VelmuruganS</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>divakarvenati</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Venati Divakar</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Contact: +91 9182848</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>+91 9182848382</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>divakarvenati@gmail.com</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>VenatiDivakar</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>vijayvs.ns</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Vijay.V.S.</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>www.vijaythedevelope</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>+919840660221</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>vijayvs.ns@gmail.com</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>VijayVS</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>vishnupriyak</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Vishnupriya</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Experience</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>vishnupriya2k14@gmail.com</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>VishnupriyaR</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>yokeshmani</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>YOKESH.M</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Phone: +91-958589686</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>9585896868</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>yokeshmani11@gmail.com</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Yokesh</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
used asyncio running successfullly in local
</commit_message>
<xml_diff>
--- a/EmployeeResumeRead/employee_resumes_data.xlsx
+++ b/EmployeeResumeRead/employee_resumes_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,192 +468,1796 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>addankilloyd</t>
+          <t>abhiverma</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Addanki Christine Ll</t>
+          <t>ABHISHEK VERMA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>9908565790 | addanki</t>
+          <t>Senior Software Engi</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>9908565790</t>
+          <t>+91 9713152685</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>addankilloyd@gmail.com</t>
+          <t>abhi8verma@gmail.com</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>AddankiChristineLloyd</t>
+          <t>AbhishekVerma</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>sivakumar.aditya</t>
+          <t>shardaadhav</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Munukutla Aditya Siv</t>
+          <t>Sharda Adhav</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Email: sivakumar.adi</t>
+          <t>Email:shardaadhav96@</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>7416877601</t>
+          <t>9370886515</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>sivakumar.aditya4@gmail.com</t>
+          <t>shardaadhav96@gmail.com</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ADITYASIVAKUMARMUNUKUTLA</t>
+          <t>AdhavShardaRangrao</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>akshaykulkarni</t>
+          <t>ajinkyaimpossible</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Akshay 11 Years of e</t>
+          <t>AJINKYA ASHOK SABLE</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>React, javascript, j</t>
+          <t>Full Stack Developer</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>9765282264</t>
+          <t>+919689343001</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>akshaykulkarni0488@gmail.com</t>
+          <t>ajinkyaimpossible@gmail.com</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>AkshayBalkrishnaKulkarni</t>
+          <t>AjinkyaAshokSable</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ambarishmamidireact</t>
+          <t>ajinkyapadwal</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ambarish Mamidi</t>
+          <t xml:space="preserve">Ajinkya D. Padwal | </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mobile: +91967635593</t>
+          <t>Technical Skills:</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>+919676355937</t>
+          <t>8459745988</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ambarishmamidireact0612@gmail.com</t>
+          <t>ajinkyapadwal5@gmail.com</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>AMBARISHMAMIDI</t>
+          <t>AjinkyaPadwal</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>amersohel</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">+91 8459416686 Amer </t>
+          <t>AKASH PHONE (+91) 80</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>amersohel4663@gmail.</t>
+          <t>EMAIL khadeakash806@</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>+91 8459416686</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>amersohel4663@gmail.com</t>
-        </is>
-      </c>
+          <t>8007326162</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>AmerSohel</t>
+          <t>AkashKhade</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>amrithraj</t>
+          <t>nairakshaynair</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Amrithraj Nalam</t>
+          <t>AKSHAY PHONE (+91) 9</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://www.linkedin</t>
+          <t>EMAIL nairakshaynair</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>+91 9908586151</t>
+          <t>9689615991</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>amrithraj879@gmail.com</t>
+          <t>nairakshaynair@gmail.co</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>AmrithrajNalam</t>
+          <t>AkshayChellath</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>shirke.amit</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>AMIT SHRIDHAR SHIRKE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>E-MAIL: shirke.amit5</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>9892981746</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>shirke.amit50@gmail.com</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>AmitShirke</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>anamikavb</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anamika Bhagannavar </t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">front End Developer </t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>8793260664</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>anamikavb284@gmail.com</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>AnamikaVikrantBhagannavar</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>apurvashinde</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>CONTACT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>APURVA RATNAPARKHI</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>+91 9175796551</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>apurvashinde57@gmail.com</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>ApurvaPratikRatnaparkhi</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>ashwinibhadane</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ASHWINI BHADANE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SOFTWARE DEVELOPER</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>ashwinibhadane09@gmail.com</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ASHWINIDEVIDASBHADANE</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>lotekarchetna</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>CHETNA PHONE (+91) 7</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>EMAIL lotekarchetna@</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>7620271806</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>lotekarchetna@gmail.co</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Chetna</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>dspansare</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>DHAIRYASHIL PANSARE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>+91 88055 55319 ⋄ Ko</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>dspansare1991@gmail.com</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>DhairyashilSanjayPansare</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>shahdhaval</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>D h a v a l S h a h</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Sr. Software Enginee</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>9408887036</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>shahdhaval0107@gmail.com</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>DhavalShah</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>dipalisingh</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Dipali Singh</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>EMAIL: dipalisingh19</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>+91 8668554363</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>dipalisingh196@gmail.com</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>DipaliSingh</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>jayssingh</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>J A Y S I N G H</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>UI and HTML Develope</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>9004128523</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>jayssingh032@gmail.com</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>JaySingh</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>kanchanshinde</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Kanchan Dattatray Sh</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Software Engineer</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>7020030298</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>kanchanshinde5495@gmail.com</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>KanchanDattatrayShinde</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>kanchaniskande</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Kanchan Kadlag</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Email: kanchaniskand</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>+91 9518574945</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>kanchaniskande1993@gmail.com</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>KanchandnyaneshwarKadlag</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>kvrsonawane</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>RESUME</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	Kavita Kewal Patade</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>9665209848</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>kvrsonawane@gmail.com</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>KavitaKewalPatade</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>ketan.valsangkar</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>WORK EXPERIENCE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Ketan Valsangkar</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>9096851512</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>ketan.valsangkar@gmail.com</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>ketan</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>skishor</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>KISHOR VYANKATESH SH</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Flat No. 33, Bldg. N</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>+919028558713</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>skishor2310@gmail.com</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>KishorVShetti</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>garjemahesh</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mahesh Arvind Garje </t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>5+ years’ experience</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>+91 7020083214</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>garjemahesh238@gmail.com</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>MaheshArvindGarje</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>bandlamudimahesh</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>RESUME</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Mahesh Bandlamudi,</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>+91 9700807171</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>bandlamudimahesh1@gmail.com</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>MaheshBandlamudi</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>anirudh.malodeofficial</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>ANIRUDH MALODE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Adaptable,Agile&amp;Rece</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>8668454903</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>anirudh.malodeofficial@gmail.com</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>MALODEANIRUDHNAMDEVRAO</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>waghmodemanisha</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Curriculum Vitae</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mrs. Manisha Hulage </t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>+91 8605903494</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>waghmodemanisha@gmail.com</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Manisha</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>mk.kamble</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>CURRICULUM VITAE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Manojkumar Balaji Ka</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>mk10.kamble@gmail.com</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>ManojkumarKambale</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>mohanrandive</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Mohan Randive</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Email:mohanrandive93</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>9158441328</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>mohanrandive93@gmail.com</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>MohanRandive</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>nagesh.kolle</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>PHONE (+91) 89755721</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NAGESH ARUN</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>8975572193</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>nagesh.kolle@gmail.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>NageshArunKolle</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>nageshangular</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Nagesh Vishwanath Sa</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>5+ years’ experience</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>+917387925918</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>nageshangular14@gmail.com</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>NageshSakhare</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>nagnathk</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>(+91) 8698183885</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>NAGNATH KARKALE</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>8698183885</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>nagnathk12@gmail.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>NagnathBalajiKarkale</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>nmtambare</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>NAMRATA TAMBARE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Email–nmtambare@gmai</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>9881913301</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>nmtambare@gmail.com</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>NamrataMangeshTambare</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>nehaninawe</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NEHA NINAWE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t xml:space="preserve">9503934643 ⋄ Pune ⋄ </t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>9503934643</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>nehaninawe7@gmail.com</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>NehaOmdeoNinawe</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>pankajpatil</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Resume</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Mr. Pankaj B Patil</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>+91 8087937671</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>pankajpatil1088@gmail.com</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>PankajBhanudasPatil</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>poojabalsaraf</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Pooja Balsaraf</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Angular developer</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>9284252853</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>poojabalsaraf64@gmail.com</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Poojabalsaraf</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>pradip</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">																</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t xml:space="preserve">																Prad</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>+91 9637316050</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>pradip8030@gmail.com</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>PradipPradhan</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>pravin.padole</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Pravin Padole</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Flat no 501,G-12, Ga</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>8855056114</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>pravin.padole15@gmail.com</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>PravinPadole</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>prem</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Prem Shankar Bharti</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Email : prem100891@g</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>+919455768438</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>prem100891@gmail.com</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>PREMSHANKARBHARTI</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>ratankavade</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>RATAN KAVADE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Senior Software Engi</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>9970344651</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>ratankavade7@gmail.com</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>RatanKavade</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>reshampawar</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Resham Vijay Pawar.</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>E-mail: reshampawar2</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>7972198086</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>reshampawar2121@gmail.com</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>ReshamVijayPawar</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>rupswagh</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Rupali Wagh</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>+91 7709210639</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>+91 7709210639</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>rupswagh2021@gmail.com</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>RupaliMarutiWagh</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>rutuja.ruke</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>PHONE (+91) 88502949</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>RUTUJA BIPIN</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>8850294958</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>rutuja.ruke9@gmail.com</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>RutujaBipinDhotre</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>samikshasajane</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Samiksha Sajane</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Software Engineer ||</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>7972068721</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>samikshasajane@gmail.com</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>SamikshaSajane</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>sandeshpangrekar</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Sandesh Pangrekar</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>E-mail: sandeshpangr</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>+91 7447713725</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>sandeshpangrekar@gmail.com</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>SandeshPangrekar</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Snjchauhan</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>SANJAY CHAUHAN</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Contact No.:+9188511</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>+918851180705</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Snjchauhan02@gmail.com</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>SANJAYCHAUHAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>stikambare</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Resume</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Tikambare Siddheshwa</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>7776877111</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>stikambare28@gmail.com</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>siddheswarVishwanathTikambare</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>smita.mulye</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Smita Mulye Mobile N</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Email-ID: smita.muly</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>8380029926</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>smita.mulye123@gmail.com</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>SmitaAnantmulye</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>snehalshahapurkar</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>snehalshahapurkar88@</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Snehal S. Shahapurka</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>8861122924</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>snehalshahapurkar88@gmail.com</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>SnehalShahapurkar</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>soniyasalampuriya</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>SONIYA SALAMPURIYA</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Email: soniyasalampu</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>+917020649379</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>soniyasalampuriya94@gmail.com</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>SoniyaSalampuriya</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sonukumar</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>SONU KUMAR</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>UI - Angular Develop</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>7058947843</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>sonukumar8021@gmail.com</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>SonuKumar</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>srpatil</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Professional Experie</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>SoftwareEngineer-Fro</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>+919766930049</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>07srpatil@gmail.com</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>SudeshPatil</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>ansarisuhail</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>SUMMARY</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>SENIOR DEVELOPER WIT</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>9773824213</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>ansarisuhail2580@gmail.com</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>SUHAILANSARI</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>sumedhaprithyani</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>WORK EXPERIENCE</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>TECHNICAL LEAD</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>sumedhaprithyani24@gmail.com</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>SumedhaPrithyani</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>shindesushma</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Sushama Shrikant Pat</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Email: shindesushma9</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>8180930668</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>shindesushma92@gmail.com</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>SushamaPatil</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>swatibhmr</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SWATI  BHAMARE </t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t xml:space="preserve">swatibhmr@gmail.com </t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>8329911620</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>swatibhmr@gmail.com</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>SwatiBhamareUIUXDeveloper</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>swati.zalavadiya</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>SWATI  ZALAVADIYA</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>swati.zalavadiya@gma</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>+91 9773101727</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>swati.zalavadiya@gmail.com</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>SwatiZalavadiya</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>tamarapu.kartik</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Tamarapu Kartik</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Hyderabad, Telangana</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>9437512801</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>tamarapu.kartik@gmail.com</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>TamarapuKartik</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>vrushankm</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Vrushank Modi</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>FRONT END DEVELOPER</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>vrushankm19@gmail.com</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>VrushankModi</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>shahzaheer</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>ZAHEER SHAH</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>FRONTEND DEVELOPER</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>+919552220876</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>shahzaheer530@gmail.com</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>ZaheerAhmadShah</t>
         </is>
       </c>
     </row>

</xml_diff>